<commit_message>
Ensuring no duplicate entries.
</commit_message>
<xml_diff>
--- a/Jail_Summaries_2020-03-10 00:00:00_to_2021-11-30 00:00:00_Generated_01-14-2022.xlsx
+++ b/Jail_Summaries_2020-03-10 00:00:00_to_2021-11-30 00:00:00_Generated_01-14-2022.xlsx
@@ -87856,13 +87856,13 @@
         <v>44470</v>
       </c>
       <c r="B572">
-        <v>806</v>
+        <v>410</v>
       </c>
       <c r="C572">
-        <v>218731.3412522409</v>
+        <v>102233.3412522409</v>
       </c>
       <c r="D572">
-        <v>115991.3344646059</v>
+        <v>99348.76303603442</v>
       </c>
     </row>
     <row r="573" spans="1:4">
@@ -87870,13 +87870,13 @@
         <v>44471</v>
       </c>
       <c r="B573">
-        <v>806</v>
+        <v>410</v>
       </c>
       <c r="C573">
-        <v>218493.5031308634</v>
+        <v>102092.5031308635</v>
       </c>
       <c r="D573">
-        <v>132982.8349118721</v>
+        <v>99711.54919758634</v>
       </c>
     </row>
     <row r="574" spans="1:4">
@@ -87884,13 +87884,13 @@
         <v>44472</v>
       </c>
       <c r="B574">
-        <v>804</v>
+        <v>408</v>
       </c>
       <c r="C574">
-        <v>219682.9983428194</v>
+        <v>102559.665009486</v>
       </c>
       <c r="D574">
-        <v>150676.6918179891</v>
+        <v>100673.5013417986</v>
       </c>
     </row>
     <row r="575" spans="1:4">
@@ -87898,13 +87898,13 @@
         <v>44473</v>
       </c>
       <c r="B575">
-        <v>806</v>
+        <v>410</v>
       </c>
       <c r="C575">
-        <v>220763.4935547753</v>
+        <v>103273.8268881086</v>
       </c>
       <c r="D575">
-        <v>167859.3337543856</v>
+        <v>101071.905182957</v>
       </c>
     </row>
     <row r="576" spans="1:4">
@@ -87912,13 +87912,13 @@
         <v>44474</v>
       </c>
       <c r="B576">
-        <v>806</v>
+        <v>411</v>
       </c>
       <c r="C576">
-        <v>219841.7221000645</v>
+        <v>102960.7221000645</v>
       </c>
       <c r="D576">
-        <v>184998.2940543948</v>
+        <v>101513.5797686805</v>
       </c>
     </row>
     <row r="577" spans="1:4">
@@ -87926,13 +87926,13 @@
         <v>44475</v>
       </c>
       <c r="B577">
-        <v>805</v>
+        <v>410</v>
       </c>
       <c r="C577">
-        <v>219231.6173120204</v>
+        <v>102553.6173120204</v>
       </c>
       <c r="D577">
-        <v>202166.9536703977</v>
+        <v>102013.9536703977</v>
       </c>
     </row>
     <row r="578" spans="1:4">
@@ -87940,13 +87940,13 @@
         <v>44476</v>
       </c>
       <c r="B578">
-        <v>803</v>
+        <v>411</v>
       </c>
       <c r="C578">
-        <v>218692.6548316686</v>
+        <v>102779.6548316686</v>
       </c>
       <c r="D578">
-        <v>219348.1900749218</v>
+        <v>102636.1900749218</v>
       </c>
     </row>
     <row r="579" spans="1:4">
@@ -87960,7 +87960,7 @@
         <v>120358.2564538809</v>
       </c>
       <c r="D579">
-        <v>205294.8922465846</v>
+        <v>105225.463675156</v>
       </c>
     </row>
     <row r="580" spans="1:4">
@@ -87974,7 +87974,7 @@
         <v>120566.7469649821</v>
       </c>
       <c r="D580">
-        <v>191305.3556514587</v>
+        <v>107864.6413657444</v>
       </c>
     </row>
     <row r="581" spans="1:4">
@@ -87988,7 +87988,7 @@
         <v>121239.2374760833</v>
       </c>
       <c r="D581">
-        <v>177241.961241925</v>
+        <v>110533.1517181155</v>
       </c>
     </row>
     <row r="582" spans="1:4">
@@ -88002,7 +88002,7 @@
         <v>121537.0137014702</v>
       </c>
       <c r="D582">
-        <v>163066.74983431</v>
+        <v>113142.1784057385</v>
       </c>
     </row>
     <row r="583" spans="1:4">
@@ -88016,7 +88016,7 @@
         <v>121383.9010379682</v>
       </c>
       <c r="D583">
-        <v>149001.3468254391</v>
+        <v>115774.0611111534</v>
       </c>
     </row>
     <row r="584" spans="1:4">
@@ -88030,7 +88030,7 @@
         <v>121355.0164446417</v>
       </c>
       <c r="D584">
-        <v>135018.9752729564</v>
+        <v>118459.9752729564</v>
       </c>
     </row>
     <row r="585" spans="1:4">

</xml_diff>